<commit_message>
ini wawancara yang bagian urg udah di buat rekapnya yah, tinggal nunggu hasil wawancara dari temen temen. ikutin aja yang punya urg
</commit_message>
<xml_diff>
--- a/Laporan/Validasi Ide.xlsx
+++ b/Laporan/Validasi Ide.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Folder HD Baru\Semester 6\Rekayasa Perangkat Lunak 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Folder HD Baru\Semester 6\Rekayasa Perangkat Lunak 2\Tugas-Besar-RPL2\Laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>PIC</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Problem Validation</t>
   </si>
   <si>
-    <t>BAHASA</t>
-  </si>
-  <si>
-    <t>CARA MENJAWAB</t>
-  </si>
-  <si>
     <t>PETUNJUK</t>
   </si>
   <si>
@@ -81,18 +75,6 @@
     <t>REKAPITULASI INTERVIEW MINGGU KE-3 APRIL 2016</t>
   </si>
   <si>
-    <t>Kurang Mengerti</t>
-  </si>
-  <si>
-    <t>Sulit</t>
-  </si>
-  <si>
-    <t>Butuh</t>
-  </si>
-  <si>
-    <t>Bisa Mengerti</t>
-  </si>
-  <si>
     <t>Kevin</t>
   </si>
   <si>
@@ -114,9 +96,6 @@
     <t>LOKASI</t>
   </si>
   <si>
-    <t>NUGRAHA</t>
-  </si>
-  <si>
     <t>Nama Interviewee</t>
   </si>
   <si>
@@ -141,25 +120,76 @@
     <t>Bukti Rekaman Validasi</t>
   </si>
   <si>
-    <t>muhammad arif</t>
-  </si>
-  <si>
-    <t>ajeng nf</t>
-  </si>
-  <si>
-    <t>syifa</t>
-  </si>
-  <si>
-    <t>ilham</t>
-  </si>
-  <si>
-    <t>Asumsi 2 : User Kesulitan Dalam Menjawab Soal Riddle</t>
-  </si>
-  <si>
     <t>Resume Rekaman</t>
   </si>
   <si>
     <t>Ya</t>
+  </si>
+  <si>
+    <t>reiga.wav</t>
+  </si>
+  <si>
+    <t>muhammad arif.wav</t>
+  </si>
+  <si>
+    <t>ajeng nf.wav</t>
+  </si>
+  <si>
+    <t>syifa.wav</t>
+  </si>
+  <si>
+    <t>ilham.wav</t>
+  </si>
+  <si>
+    <t>0.27</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>Tidak</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>Asumsi 2 : User Menginginkan soal Riddle yang Lebih Dapat Dimengerti</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>SOAL KURANG DIMENGERTI</t>
+  </si>
+  <si>
+    <t>BAHASA INDONESIA</t>
   </si>
 </sst>
 </file>
@@ -275,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,6 +319,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -301,35 +361,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,299 +680,358 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="9.140625" style="11"/>
-    <col min="3" max="3" width="17.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="11" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="18" style="11" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="19" style="9" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="9.140625" style="6"/>
+    <col min="3" max="3" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="18" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="19" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="2:16" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="2:16" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18" t="s">
+      <c r="I10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
-        <v>1</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="H13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
+        <v>6</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
         <v>7</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
-        <v>2</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
         <v>8</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
-        <v>3</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
         <v>9</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
-        <v>4</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="P17" s="19"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
         <v>10</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-    </row>
-    <row r="13" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12">
-        <v>6</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
-        <v>7</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
-        <v>8</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="P16" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
-        <v>9</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="P17" s="10"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
-        <v>10</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="P18" s="10"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="P18" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
+    <mergeCell ref="E3:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G3:H5"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D8"/>
@@ -951,12 +1043,6 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
-    <mergeCell ref="P16:P18"/>
-    <mergeCell ref="E3:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G3:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -965,85 +1051,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="B2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="2" t="s">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
+      <c r="D5" s="14">
+        <v>5</v>
+      </c>
+      <c r="E5" s="14">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1053,20 +1141,20 @@
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1074,90 +1162,108 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>27</v>
+      <c r="B10" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4">
+        <v>18</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="14">
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>4</v>
@@ -1165,11 +1271,6 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
urang udah nambahin riskiest assumption di file excel
</commit_message>
<xml_diff>
--- a/Laporan/Validasi Ide.xlsx
+++ b/Laporan/Validasi Ide.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
-    <sheet name="Resume Rekaman" sheetId="2" r:id="rId1"/>
-    <sheet name="Rekapitulasi Interview" sheetId="1" r:id="rId2"/>
+    <sheet name="Masalah &amp; Riskiest Assumption" sheetId="3" r:id="rId1"/>
+    <sheet name="Resume Rekaman" sheetId="2" r:id="rId2"/>
+    <sheet name="Rekapitulasi Interview" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>PIC</t>
   </si>
@@ -190,6 +191,33 @@
   </si>
   <si>
     <t>BAHASA INDONESIA</t>
+  </si>
+  <si>
+    <t>Masalah belum ada  aplikasi riddle bahasa indonesia</t>
+  </si>
+  <si>
+    <t>Masalah soal riddle yang cenderung sulit dipahami</t>
+  </si>
+  <si>
+    <t>Masalah Minimnya Petunjuk didalam permainan Riddle</t>
+  </si>
+  <si>
+    <t>kebanyakan aplikasi permainan riddle menggunakan bahasa Inggris</t>
+  </si>
+  <si>
+    <t>Riddle membutuhkan kemampuan analisa yang kuat</t>
+  </si>
+  <si>
+    <t>Petunjuk di dalam riddle itu penting</t>
+  </si>
+  <si>
+    <t>Riddle berbahasa indonesia masih dikenal dikalangan forum di internet (misal : Kaskus)</t>
+  </si>
+  <si>
+    <t>Tidak semua orang bisa memahami sehingga tidak semua orang tertarik untuk menjawab Riddle</t>
+  </si>
+  <si>
+    <t>Riddle masih belum begitu dikenal di Indonesia</t>
   </si>
 </sst>
 </file>
@@ -214,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,21 +365,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -361,8 +398,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,9 +715,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="2:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -700,67 +808,67 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="2:16" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="11" t="s">
         <v>28</v>
       </c>
@@ -775,9 +883,9 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="12" t="s">
         <v>29</v>
       </c>
@@ -798,9 +906,9 @@
       </c>
     </row>
     <row r="8" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -995,7 +1103,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="P16" s="19"/>
+      <c r="P16" s="9"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
@@ -1009,7 +1117,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="P17" s="19"/>
+      <c r="P17" s="9"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
@@ -1023,15 +1131,10 @@
       <c r="H18" s="7"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="P18" s="19"/>
+      <c r="P18" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E3:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G3:H5"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D8"/>
@@ -1043,13 +1146,18 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
+    <mergeCell ref="E3:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G3:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J11"/>
   <sheetViews>
@@ -1067,50 +1175,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="2" t="s">
         <v>54</v>
       </c>
@@ -1122,16 +1230,16 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="15">
         <v>5</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="15">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1151,10 +1259,10 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1172,10 +1280,10 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1193,10 +1301,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1214,10 +1322,10 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1235,14 +1343,14 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14">
+      <c r="D10" s="16"/>
+      <c r="E10" s="15">
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1256,12 +1364,12 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>